<commit_message>
estructura inical version final
</commit_message>
<xml_diff>
--- a/Documentacion/PlanificacionProyecto1.xlsx
+++ b/Documentacion/PlanificacionProyecto1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\XAMP\DAW\Proyectos\PROYECTO1\Documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
   <si>
     <t>Miercoles</t>
   </si>
@@ -102,6 +102,12 @@
   </si>
   <si>
     <t>SI ES NECESARIO: crear mas php</t>
+  </si>
+  <si>
+    <t>PHP: login</t>
+  </si>
+  <si>
+    <t>CSS: ventanaModal</t>
   </si>
 </sst>
 </file>
@@ -169,6 +175,114 @@
   </cellStyles>
   <dxfs count="15">
     <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <strike val="0"/>
         <outline val="0"/>
@@ -187,114 +301,6 @@
         </patternFill>
       </fill>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -310,7 +316,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="A4:F12" headerRowDxfId="0" dataDxfId="2" totalsRowDxfId="1" headerRowCellStyle="Texto explicativo" dataCellStyle="Texto explicativo">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="A4:F12" headerRowDxfId="14" dataDxfId="13" totalsRowDxfId="12">
   <autoFilter ref="A4:F12">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -320,12 +326,12 @@
     <filterColumn colId="5" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="6">
-    <tableColumn id="1" name="Miercoles" totalsRowLabel="Total" dataDxfId="8" totalsRowDxfId="9"/>
-    <tableColumn id="2" name="Jueves" dataDxfId="7" totalsRowDxfId="10"/>
-    <tableColumn id="3" name="Viernes" dataDxfId="6" totalsRowDxfId="11"/>
-    <tableColumn id="4" name="Lunes" dataDxfId="5" totalsRowDxfId="12"/>
-    <tableColumn id="5" name="Martes" dataDxfId="4" totalsRowDxfId="13"/>
-    <tableColumn id="6" name="Miercoles2" totalsRowFunction="count" dataDxfId="3" totalsRowDxfId="14"/>
+    <tableColumn id="1" name="Miercoles" totalsRowLabel="Total" dataDxfId="11" totalsRowDxfId="10"/>
+    <tableColumn id="2" name="Jueves" dataDxfId="9" totalsRowDxfId="8"/>
+    <tableColumn id="3" name="Viernes" dataDxfId="7" totalsRowDxfId="6"/>
+    <tableColumn id="4" name="Lunes" dataDxfId="5" totalsRowDxfId="4"/>
+    <tableColumn id="5" name="Martes" dataDxfId="3" totalsRowDxfId="2"/>
+    <tableColumn id="6" name="Miercoles2" totalsRowFunction="count" dataDxfId="1" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -597,7 +603,7 @@
   <dimension ref="A4:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -668,11 +674,15 @@
         <v>10</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="1"/>
       <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
+      <c r="E7" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>